<commit_message>
Basiclly completed, wit rank plot unplotted for technical reasons.
</commit_message>
<xml_diff>
--- a/Data/vulnerabilityAssessmentData.xlsx
+++ b/Data/vulnerabilityAssessmentData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Liuyue/Documents/F-CNVul/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E710747-4AA7-0447-A86C-8D3C0445E4DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF2C115-3BFE-C142-A29C-1D89132115A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="0" windowWidth="40040" windowHeight="23040" activeTab="1" xr2:uid="{C3CB43DF-AD04-A345-AFD0-1953B0F0A34C}"/>
+    <workbookView xWindow="920" yWindow="0" windowWidth="40040" windowHeight="23040" xr2:uid="{C3CB43DF-AD04-A345-AFD0-1953B0F0A34C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -987,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA250CB-DF44-644E-8EF4-21481D438232}">
   <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N75" sqref="N75"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1328,7 +1328,7 @@
         <v>JiangSu</v>
       </c>
       <c r="D7">
-        <v>210000</v>
+        <v>320000</v>
       </c>
       <c r="E7" s="1">
         <v>9.488550743628382</v>
@@ -1890,7 +1890,7 @@
         <v>JiangSu</v>
       </c>
       <c r="D18">
-        <v>210000</v>
+        <v>320000</v>
       </c>
       <c r="E18" s="1">
         <v>8.69469538683542</v>
@@ -2452,7 +2452,7 @@
         <v>JiangSu</v>
       </c>
       <c r="D29">
-        <v>210000</v>
+        <v>320000</v>
       </c>
       <c r="E29" s="1">
         <v>9.8946299677490916</v>
@@ -3014,7 +3014,7 @@
         <v>JiangSu</v>
       </c>
       <c r="D40">
-        <v>210000</v>
+        <v>320000</v>
       </c>
       <c r="E40" s="1">
         <v>10.00289617391001</v>
@@ -3576,7 +3576,7 @@
         <v>JiangSu</v>
       </c>
       <c r="D51">
-        <v>210000</v>
+        <v>320000</v>
       </c>
       <c r="E51" s="1">
         <v>9.8992225088905936</v>
@@ -4138,7 +4138,7 @@
         <v>JiangSu</v>
       </c>
       <c r="D62">
-        <v>210000</v>
+        <v>320000</v>
       </c>
       <c r="E62" s="1">
         <v>10.286288771549463</v>
@@ -4443,7 +4443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A967A321-35B0-9643-A83C-92DC58311C4C}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>